<commit_message>
add libraries for read data from file excel
</commit_message>
<xml_diff>
--- a/src/main/resources/BookSelenium.xlsx
+++ b/src/main/resources/BookSelenium.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\seleniumproject\selenium_minh\src\main\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="21075" windowHeight="9795" activeTab="1"/>
   </bookViews>
@@ -23,12 +18,12 @@
     <definedName name="Quảng_Ngãi">Sheet1!$L$2:$L$6</definedName>
     <definedName name="Sài_Gòn">Sheet1!$H$2:$H$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="28">
   <si>
     <t>Depart Date</t>
   </si>
@@ -97,13 +92,28 @@
   </si>
   <si>
     <t>Soft bed with air conditioner</t>
+  </si>
+  <si>
+    <t>4/26/2021</t>
+  </si>
+  <si>
+    <t>4/27/2021</t>
+  </si>
+  <si>
+    <t>4/28/2021</t>
+  </si>
+  <si>
+    <t>4/29/2021</t>
+  </si>
+  <si>
+    <t>4/30/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +128,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,11 +156,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -205,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -508,7 +528,7 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f ca="1">TODAY()+3</f>
-        <v>44311</v>
+        <v>44312</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -544,7 +564,7 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f ca="1">TODAY()+4</f>
-        <v>44312</v>
+        <v>44313</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -580,7 +600,7 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f ca="1">TODAY()+5</f>
-        <v>44313</v>
+        <v>44314</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -616,7 +636,7 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f ca="1">TODAY()+6</f>
-        <v>44314</v>
+        <v>44315</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -649,7 +669,7 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f ca="1">TODAY()+7</f>
-        <v>44315</v>
+        <v>44316</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -670,7 +690,7 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f ca="1">TODAY()+8</f>
-        <v>44316</v>
+        <v>44317</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -688,7 +708,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f ca="1">TODAY()+9</f>
-        <v>44317</v>
+        <v>44318</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
@@ -712,7 +732,7 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f ca="1">TODAY()+10</f>
-        <v>44318</v>
+        <v>44319</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -736,7 +756,7 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f ca="1">TODAY()+11</f>
-        <v>44319</v>
+        <v>44320</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
@@ -760,7 +780,7 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f ca="1">TODAY()+12</f>
-        <v>44320</v>
+        <v>44321</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -784,7 +804,7 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f ca="1">TODAY()+13</f>
-        <v>44321</v>
+        <v>44322</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
@@ -808,7 +828,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f ca="1">TODAY()+14</f>
-        <v>44322</v>
+        <v>44323</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
@@ -832,7 +852,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f ca="1">TODAY()+15</f>
-        <v>44323</v>
+        <v>44324</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -856,7 +876,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f ca="1">TODAY()+16</f>
-        <v>44324</v>
+        <v>44325</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -877,7 +897,7 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f ca="1">TODAY()+17</f>
-        <v>44325</v>
+        <v>44326</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
@@ -898,7 +918,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f ca="1">TODAY()+18</f>
-        <v>44326</v>
+        <v>44327</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -919,7 +939,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f ca="1">TODAY()+19</f>
-        <v>44327</v>
+        <v>44328</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
@@ -1008,7 +1028,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,8 +1058,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>44312</v>
+      <c r="A2" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1055,8 +1075,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>44312</v>
+      <c r="A3" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1072,8 +1092,8 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>44313</v>
+      <c r="A4" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1089,8 +1109,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>44314</v>
+      <c r="A5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1106,8 +1126,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>44315</v>
+      <c r="A6" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -1123,8 +1143,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>44316</v>
+      <c r="A7" s="5">
+        <v>44201</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -1140,8 +1160,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>44317</v>
+      <c r="A8" s="4">
+        <v>44232</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1157,8 +1177,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>44318</v>
+      <c r="A9" s="4">
+        <v>44260</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -1174,8 +1194,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>44319</v>
+      <c r="A10" s="4">
+        <v>44291</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -1191,8 +1211,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>44320</v>
+      <c r="A11" s="4">
+        <v>44321</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1208,8 +1228,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>44321</v>
+      <c r="A12" s="4">
+        <v>44352</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1225,8 +1245,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>44322</v>
+      <c r="A13" s="4">
+        <v>44382</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -1242,8 +1262,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>44323</v>
+      <c r="A14" s="4">
+        <v>44413</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1259,8 +1279,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>44324</v>
+      <c r="A15" s="4">
+        <v>44444</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -1276,8 +1296,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>44325</v>
+      <c r="A16" s="4">
+        <v>44474</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1293,8 +1313,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>44326</v>
+      <c r="A17" s="4">
+        <v>44505</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1310,8 +1330,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>44327</v>
+      <c r="A18" s="4">
+        <v>44535</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -1328,5 +1348,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>